<commit_message>
Create role management system
Co-authored-by: Anto Wiranto <antowrnto11@gmail.com>
</commit_message>
<xml_diff>
--- a/storage/AgingRate.xlsx
+++ b/storage/AgingRate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\tjsl\storage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FA1F2C6A-7769-4456-8759-3F25B79ED44E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D6C201F-A1A4-4738-BA98-B1BCE7B9F740}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130" xr2:uid="{E04815D7-E530-4992-B64A-1CE12D86837B}"/>
   </bookViews>
@@ -752,7 +752,7 @@
   <dimension ref="A1:Z31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -2043,7 +2043,10 @@
       <c r="W13" s="23"/>
       <c r="X13" s="23"/>
       <c r="Y13" s="23"/>
-      <c r="Z13" s="23"/>
+      <c r="Z13" s="23" t="e">
+        <f>AVERAGE(C13:Y13)</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="14" spans="1:26" ht="30.75" thickBot="1">
       <c r="B14" s="22" t="s">
@@ -2072,7 +2075,10 @@
       <c r="W14" s="24"/>
       <c r="X14" s="24"/>
       <c r="Y14" s="24"/>
-      <c r="Z14" s="23"/>
+      <c r="Z14" s="23" t="e">
+        <f>AVERAGE(C14:Y14)</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="15" spans="1:26" ht="30.75" thickBot="1">
       <c r="B15" s="22" t="s">
@@ -2101,7 +2107,10 @@
       <c r="W15" s="23"/>
       <c r="X15" s="24"/>
       <c r="Y15" s="24"/>
-      <c r="Z15" s="23"/>
+      <c r="Z15" s="23" t="e">
+        <f>AVERAGE(C15:Y15)</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="18" spans="1:20" ht="45">
       <c r="A18" s="27"/>

</xml_diff>